<commit_message>
Minor updates to v0.3 BOM and silkscreen
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/v0.3_bom.xlsx
+++ b/reference/hardware/v0.3/v0.3_bom.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25711"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/speeduino/reference/hardware/v0.3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -53,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="199">
   <si>
     <t>QTY</t>
   </si>
@@ -187,9 +192,6 @@
     <t>399-9714-ND</t>
   </si>
   <si>
-    <t>5.6v 1w</t>
-  </si>
-  <si>
     <t>DIODE ZENER 5.6V 3W AXIAL</t>
   </si>
   <si>
@@ -253,9 +255,6 @@
     <t>Jumper</t>
   </si>
   <si>
-    <t>0.100 Pin Header</t>
-  </si>
-  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
@@ -304,9 +303,6 @@
     <t>RNF14FTD470RCT-ND</t>
   </si>
   <si>
-    <t>2.49k</t>
-  </si>
-  <si>
     <t>RES 2.49K OHM 0.25W 0.1% METAL FILM</t>
   </si>
   <si>
@@ -322,9 +318,6 @@
     <t>985-1047-1-ND</t>
   </si>
   <si>
-    <t>3.9k</t>
-  </si>
-  <si>
     <t>RES 3.9K OHM 1/4W 0.1% METAL FILM AXL</t>
   </si>
   <si>
@@ -334,9 +327,6 @@
     <t>3.9KADCT-ND</t>
   </si>
   <si>
-    <t>1.0k</t>
-  </si>
-  <si>
     <t>RES 1K OHM 1/4W 0.1% METAL FILM AXL</t>
   </si>
   <si>
@@ -565,9 +555,6 @@
     <t>24LC512-I/P-ND</t>
   </si>
   <si>
-    <t>24LC512</t>
-  </si>
-  <si>
     <t>IC EEPROM 512KBIT 400KHZ 8DIP</t>
   </si>
   <si>
@@ -592,9 +579,6 @@
     <t>Screw Terminal block</t>
   </si>
   <si>
-    <t>Terminal Block</t>
-  </si>
-  <si>
     <t>OSTTA020161</t>
   </si>
   <si>
@@ -620,6 +604,57 @@
   </si>
   <si>
     <t>Digikey import</t>
+  </si>
+  <si>
+    <t>Dual Terminal Block</t>
+  </si>
+  <si>
+    <t>40 POS 0.100 Pin Header</t>
+  </si>
+  <si>
+    <t>62A MOSFET N-CH</t>
+  </si>
+  <si>
+    <t>1-Bar MAP sensor</t>
+  </si>
+  <si>
+    <t>512Kb EEPROM</t>
+  </si>
+  <si>
+    <t>IC Socket</t>
+  </si>
+  <si>
+    <t>General Description</t>
+  </si>
+  <si>
+    <t>0.1% 3.9k</t>
+  </si>
+  <si>
+    <t>0.1% 1.0k</t>
+  </si>
+  <si>
+    <t>0.1% 2.49k</t>
+  </si>
+  <si>
+    <t>1N5919BG Zener</t>
+  </si>
+  <si>
+    <t>1N5818-TP Schottky</t>
+  </si>
+  <si>
+    <t>IC1,2</t>
+  </si>
+  <si>
+    <t>TC4424EPA</t>
+  </si>
+  <si>
+    <t>IC MOSFET DVR 3A DUAL HS 8-DIP</t>
+  </si>
+  <si>
+    <t>8-DIP</t>
+  </si>
+  <si>
+    <t>TC4424EPA-ND</t>
   </si>
 </sst>
 </file>
@@ -694,7 +729,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -723,6 +758,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -787,7 +828,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -827,8 +868,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -892,17 +940,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="46">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -940,11 +994,23 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1273,13 +1339,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="69.83203125" customWidth="1"/>
@@ -1289,14 +1355,15 @@
     <col min="9" max="9" width="28" customWidth="1"/>
     <col min="12" max="12" width="47.83203125" customWidth="1"/>
     <col min="13" max="13" width="27.33203125" customWidth="1"/>
+    <col min="14" max="14" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27" thickBot="1">
+    <row r="1" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1328,11 +1395,14 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="N1" s="23" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16" thickBot="1">
+    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -1349,14 +1419,18 @@
         <f>IF(NOT(I2=""),A2&amp;","&amp;I2,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="27" thickBot="1">
+      <c r="N2" t="str">
+        <f>A2&amp;"x "&amp;C2</f>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
@@ -1388,17 +1462,21 @@
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4" t="str">
-        <f t="shared" ref="M3:M49" si="1">IF(NOT(I3=""),A3&amp;","&amp;I3,"")</f>
+        <f t="shared" ref="M3:M50" si="1">IF(NOT(I3=""),A3&amp;","&amp;I3,"")</f>
         <v>1,478-1842-ND</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="16" thickBot="1">
+      <c r="N3" t="str">
+        <f>"Capacitor - " &amp;A3&amp;"x "&amp;C3</f>
+        <v>Capacitor - 1x 10uF</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
@@ -1433,14 +1511,18 @@
         <f t="shared" si="1"/>
         <v>5,399-4288-ND</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="16" thickBot="1">
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N10" si="2">"Capacitor - " &amp;A4&amp;"x "&amp;C4</f>
+        <v>Capacitor - 5x 0.22uF</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>23</v>
@@ -1475,14 +1557,18 @@
         <f t="shared" si="1"/>
         <v>7,399-4264-ND</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="27" thickBot="1">
+      <c r="N5" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 7x 0.1uF / 100nF</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>27</v>
@@ -1517,14 +1603,18 @@
         <f t="shared" si="1"/>
         <v>1,478-1910-ND</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="27" thickBot="1">
+      <c r="N6" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 1x 47uF</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
-        <f t="shared" ref="A7:A9" si="2">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
+        <f t="shared" ref="A7:A9" si="3">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>31</v>
@@ -1559,14 +1649,18 @@
         <f t="shared" si="1"/>
         <v>1,445-5312-ND</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="16" thickBot="1">
+      <c r="N7" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 1x 0.33uF</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>36</v>
@@ -1601,14 +1695,18 @@
         <f t="shared" si="1"/>
         <v>1,399-4148-ND</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="16" thickBot="1">
+      <c r="N8" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 1x 0.01uF</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>40</v>
@@ -1643,20 +1741,24 @@
         <f t="shared" si="1"/>
         <v>3,399-9714-ND</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="16" thickBot="1">
+      <c r="N9" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 3x 1uF</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>19</v>
@@ -1666,10 +1768,10 @@
         <v>20</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="J10" s="5">
         <v>0.25</v>
@@ -1683,8 +1785,12 @@
         <f t="shared" si="1"/>
         <v>1,399-4243-ND</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="16" thickBot="1">
+      <c r="N10" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 1x 4.7nF</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -1702,7 +1808,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="16" thickBot="1">
+    <row r="12" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -1720,34 +1826,34 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="40" thickBot="1">
+    <row r="13" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="J13" s="5">
         <v>0.34</v>
@@ -1761,35 +1867,39 @@
         <f t="shared" si="1"/>
         <v>1,1N5919BGOS-ND</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="40" thickBot="1">
+      <c r="N13" t="str">
+        <f>"Diode - " &amp;A13&amp;"x "&amp;C13</f>
+        <v>Diode - 1x 1N5919BG Zener</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="3">
         <v>18</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="J14" s="5">
         <v>0.27</v>
@@ -1803,29 +1913,33 @@
         <f t="shared" si="1"/>
         <v>12,1N5818-TPCT-ND</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="16" thickBot="1">
+      <c r="N14" t="str">
+        <f t="shared" ref="N14:N16" si="4">"Diode - " &amp;A14&amp;"x "&amp;C14</f>
+        <v>Diode - 12x 1N5818-TP Schottky</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J15" s="5">
         <v>0.47</v>
@@ -1839,35 +1953,39 @@
         <f t="shared" si="1"/>
         <v>8,160-1139-ND</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="40" thickBot="1">
+      <c r="N15" t="str">
+        <f t="shared" si="4"/>
+        <v>Diode - 8x LED-Red</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F16" s="3">
         <v>13</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="J16" s="5">
         <v>0.11</v>
@@ -1881,8 +1999,12 @@
         <f t="shared" si="1"/>
         <v>4,1N4004-TPMSCT-ND</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="16" thickBot="1">
+      <c r="N16" t="str">
+        <f t="shared" si="4"/>
+        <v>Diode - 4x 1N4004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -1899,8 +2021,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="16" thickBot="1">
+      <c r="N17" t="str">
+        <f t="shared" ref="N17:N45" si="5">A17&amp;"x "&amp;C17</f>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -1917,8 +2043,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="16" thickBot="1">
+      <c r="N18" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -1935,34 +2065,38 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="27" thickBot="1">
+      <c r="N19" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="F20" s="3">
         <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="J20" s="5">
         <v>0.72</v>
@@ -1976,8 +2110,12 @@
         <f t="shared" si="1"/>
         <v>1,P7307-ND</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="16" thickBot="1">
+      <c r="N20" t="str">
+        <f t="shared" si="5"/>
+        <v>1x Surge Protection</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
@@ -1994,30 +2132,34 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="40" thickBot="1">
+      <c r="N21" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="J22" s="3">
         <v>0.40200000000000002</v>
@@ -2027,32 +2169,36 @@
         <v>5.6280000000000001</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="M22" s="4" t="str">
         <f t="shared" si="1"/>
         <v>14,ED2561-ND</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="16" thickBot="1">
+      <c r="N22" t="str">
+        <f>A22&amp;"x "&amp;C22</f>
+        <v>14x Dual Terminal Block</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="J23" s="5">
         <v>0.1</v>
@@ -2066,32 +2212,36 @@
         <f t="shared" si="1"/>
         <v>5,3M9580-ND</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="40" thickBot="1">
+      <c r="N23" t="str">
+        <f t="shared" si="5"/>
+        <v>5x Jumper</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>66</v>
+        <v>183</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3">
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="J24" s="6">
         <v>0.56000000000000005</v>
@@ -2105,8 +2255,12 @@
         <f t="shared" si="1"/>
         <v>1,S1012EC-40-ND</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="16" thickBot="1">
+      <c r="N24" t="str">
+        <f t="shared" si="5"/>
+        <v>1x 40 POS 0.100 Pin Header</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
@@ -2123,8 +2277,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="16" thickBot="1">
+      <c r="N25" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
@@ -2141,35 +2299,39 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="27" thickBot="1">
+      <c r="N26" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F27" s="3">
         <v>8</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J27" s="6">
         <v>1.51</v>
@@ -2183,8 +2345,12 @@
         <f t="shared" si="1"/>
         <v>8,497-5896-5-ND</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="16" thickBot="1">
+      <c r="N27" t="str">
+        <f t="shared" si="5"/>
+        <v>8x 62A MOSFET N-CH</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
@@ -2202,7 +2368,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16" thickBot="1">
+    <row r="29" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
@@ -2220,38 +2386,38 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="16" thickBot="1">
+    <row r="30" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3">
         <v>7</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="J30" s="5">
         <v>0.08</v>
       </c>
       <c r="K30" s="6">
-        <f t="shared" ref="K30:K38" si="3">J30*A30</f>
+        <f t="shared" ref="K30:K38" si="6">J30*A30</f>
         <v>0.4</v>
       </c>
       <c r="L30" s="4"/>
@@ -2259,39 +2425,43 @@
         <f t="shared" si="1"/>
         <v>5,10.0KXBK-ND</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="16" thickBot="1">
+      <c r="N30" t="str">
+        <f>"Resistor - " &amp; A30&amp;"x "&amp;C30</f>
+        <v>Resistor - 5x 10k</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21">
         <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3">
         <v>32</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J31" s="5">
         <v>0.06</v>
       </c>
       <c r="K31" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.72</v>
       </c>
       <c r="L31" s="4"/>
@@ -2299,81 +2469,89 @@
         <f t="shared" si="1"/>
         <v>12,1.00KXBK-ND</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="27" thickBot="1">
+      <c r="N31" t="str">
+        <f t="shared" ref="N31:N38" si="7">"Resistor - " &amp; A31&amp;"x "&amp;C31</f>
+        <v>Resistor - 12x 1k</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C32" s="14">
         <v>680</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="14">
         <v>17</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J32" s="15">
         <v>0.14000000000000001</v>
       </c>
       <c r="K32" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.1200000000000001</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="M32" s="4" t="str">
         <f t="shared" si="1"/>
         <v>8,2.43KXBK-ND</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" ht="40" thickBot="1">
+      <c r="N32" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 8x 680</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C33" s="3">
         <v>470</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3">
         <v>9</v>
       </c>
       <c r="G33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="J33" s="5">
         <v>0.11</v>
       </c>
       <c r="K33" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.66</v>
       </c>
       <c r="L33" s="4"/>
@@ -2381,40 +2559,44 @@
         <f t="shared" si="1"/>
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" ht="40" thickBot="1">
+      <c r="N33" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 6x 470</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F34" s="3">
         <v>3</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J34" s="5">
         <v>1.92</v>
       </c>
       <c r="K34" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.84</v>
       </c>
       <c r="L34" s="4"/>
@@ -2422,121 +2604,133 @@
         <f t="shared" si="1"/>
         <v>2,985-1047-1-ND</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="16" thickBot="1">
+      <c r="N34" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 2x 0.1% 2.49k</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>89</v>
+        <v>189</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3">
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J35" s="5">
         <v>0.46</v>
       </c>
       <c r="K35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.46</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="M35" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,3.9KADCT-ND</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" ht="16" thickBot="1">
+      <c r="N35" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 1x 0.1% 3.9k</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>93</v>
+        <v>190</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3">
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J36" s="5">
         <v>0.46</v>
       </c>
       <c r="K36" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.46</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="M36" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,1KADCT-ND</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="16" thickBot="1">
+      <c r="N36" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 1x 0.1% 1.0k</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21">
-        <f t="shared" ref="A37:A38" si="4">LEN(B37)-LEN(SUBSTITUTE(B37,",",""))+1</f>
+        <f t="shared" ref="A37:A38" si="8">LEN(B37)-LEN(SUBSTITUTE(B37,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3">
         <v>17</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J37" s="5">
         <v>0.1</v>
       </c>
       <c r="K37" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="L37" s="4"/>
@@ -2544,39 +2738,43 @@
         <f t="shared" si="1"/>
         <v>12,100KXBK-ND</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" ht="27" thickBot="1">
+      <c r="N37" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 12x 100k</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C38" s="3">
         <v>160</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3">
         <v>4</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J38" s="5">
         <v>0.27</v>
       </c>
       <c r="K38" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.08</v>
       </c>
       <c r="L38" s="4"/>
@@ -2584,8 +2782,12 @@
         <f t="shared" si="1"/>
         <v>4,160YCT-ND</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="16" thickBot="1">
+      <c r="N38" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 4x 160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
@@ -2603,7 +2805,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="16" thickBot="1">
+    <row r="40" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3"/>
@@ -2621,33 +2823,33 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="40" thickBot="1">
+    <row r="41" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21">
         <v>1</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F41" s="3">
         <v>2</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J41" s="5">
         <v>1.68</v>
@@ -2661,30 +2863,36 @@
         <f t="shared" si="1"/>
         <v>1,LM2940T-5.0/NOPB</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="40" thickBot="1">
+      <c r="N41" t="str">
+        <f t="shared" si="5"/>
+        <v>1x LM2940T-5.0/NOPB</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="D42" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F42" s="3">
         <v>1</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="J42" s="6">
         <v>15.41</v>
@@ -2698,247 +2906,304 @@
         <f t="shared" si="1"/>
         <v>1,MPX4250AP-ND</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="27" thickBot="1">
-      <c r="A43" s="21">
-        <v>1</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>171</v>
+      <c r="N42" t="str">
+        <f t="shared" si="5"/>
+        <v>1x 1-Bar MAP sensor</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="26">
+        <v>2</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>196</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="J43" s="6">
-        <v>1.61</v>
+        <v>197</v>
+      </c>
+      <c r="F43" s="14">
+        <v>2</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="J43" s="27">
+        <v>2.92</v>
       </c>
       <c r="K43" s="6">
         <f>J43*A43</f>
+        <v>5.84</v>
+      </c>
+      <c r="L43" s="13"/>
+      <c r="M43" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>2,TC4424EPA-ND</v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="5"/>
+        <v>2x TC4424EPA</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="21">
+        <v>1</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J44" s="6">
         <v>1.61</v>
-      </c>
-      <c r="L43" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="M43" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>1,24LC512-I/P-ND</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="16" thickBot="1">
-      <c r="A44" s="21">
-        <v>3</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J44" s="6">
-        <v>0.5</v>
       </c>
       <c r="K44" s="6">
         <f>J44*A44</f>
-        <v>1.5</v>
-      </c>
-      <c r="L44" s="4"/>
+        <v>1.61</v>
+      </c>
+      <c r="L44" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="M44" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>3,AE10011-ND</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="16" thickBot="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="3"/>
+        <v>1,24LC512-I/P-ND</v>
+      </c>
+      <c r="N44" t="str">
+        <f t="shared" si="5"/>
+        <v>1x 512Kb EEPROM</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="21">
+        <v>3</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J45" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="K45" s="6">
+        <f>J45*A45</f>
+        <v>1.5</v>
+      </c>
+      <c r="L45" s="4"/>
       <c r="M45" s="4" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="16" thickBot="1">
-      <c r="A46" s="18">
-        <v>0</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>149</v>
-      </c>
+        <v>3,AE10011-ND</v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" si="5"/>
+        <v>3x IC Socket</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="4"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="3">
-        <v>1</v>
-      </c>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6">
-        <f>J46*A46</f>
-        <v>0</v>
-      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="11"/>
       <c r="L46" s="11"/>
       <c r="M46" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="16" thickBot="1">
-      <c r="A47" s="18"/>
-      <c r="B47" s="4"/>
+    <row r="47" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18">
+        <v>0</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="11"/>
+      <c r="F47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6">
+        <f>J47*A47</f>
+        <v>0</v>
+      </c>
       <c r="L47" s="11"/>
       <c r="M47" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="16" thickBot="1">
+    <row r="48" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
-      <c r="B48" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="B48" s="4"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="9"/>
+      <c r="F48" s="4"/>
       <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
+      <c r="H48" s="10"/>
       <c r="I48" s="3"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="4"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
       <c r="M48" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="16" thickBot="1">
-      <c r="A49" s="18">
-        <v>1</v>
-      </c>
+    <row r="49" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
       <c r="B49" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>114</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="3">
-        <v>1</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="F49" s="9"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
       <c r="I49" s="3"/>
-      <c r="J49" s="6">
-        <v>15</v>
-      </c>
-      <c r="K49" s="6">
-        <f>J49*A49</f>
-        <v>15</v>
-      </c>
+      <c r="J49" s="4"/>
+      <c r="K49" s="3"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="27" thickBot="1">
+    <row r="50" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18">
         <v>1</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C50" s="3"/>
+        <v>149</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="J50" s="3">
-        <v>61.65</v>
-      </c>
-      <c r="K50" s="6"/>
-      <c r="L50" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="16" thickBot="1">
-      <c r="A51" s="18"/>
-      <c r="B51" s="4"/>
+      <c r="F50" s="3">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="6">
+        <v>15</v>
+      </c>
+      <c r="K50" s="6">
+        <f>J50*A50</f>
+        <v>15</v>
+      </c>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18">
+        <v>1</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="I51" s="24"/>
-      <c r="J51" s="1" t="s">
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J51" s="3">
+        <v>61.65</v>
+      </c>
+      <c r="K51" s="6"/>
+      <c r="L51" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="K51" s="12">
-        <f>SUM(K2:K50)</f>
-        <v>83.828000000000003</v>
-      </c>
-      <c r="L51" s="11" t="s">
-        <v>112</v>
+      <c r="I52" s="25"/>
+      <c r="J52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K52" s="12">
+        <f>SUM(K2:K51)</f>
+        <v>89.668000000000006</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H52:I52"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -2958,10 +3223,5 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="36" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId13"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix incorrect part number on 680 Ohm resistors
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/v0.3_bom.xlsx
+++ b/reference/hardware/v0.3/v0.3_bom.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25711"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/speeduino/reference/hardware/v0.3/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20940" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Full Kit" sheetId="1" r:id="rId1"/>
+    <sheet name="2 Channel" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -57,8 +53,42 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Josh Stewart</author>
+  </authors>
+  <commentList>
+    <comment ref="B34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Josh Stewart:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Optional 3rd one for a spare ADC</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="209">
   <si>
     <t>QTY</t>
   </si>
@@ -285,12 +315,6 @@
     <t>1.00KXBK-ND</t>
   </si>
   <si>
-    <t>MFR-25FBF52-2K43</t>
-  </si>
-  <si>
-    <t>2.43KXBK-ND</t>
-  </si>
-  <si>
     <t>RES METAL FILM 1/4W 470 OHM 1% AXIAL</t>
   </si>
   <si>
@@ -408,9 +432,6 @@
     <t>R21</t>
   </si>
   <si>
-    <t>RES 680 OHM 1/4W 1% AXIAL</t>
-  </si>
-  <si>
     <t>R25,27,31,32</t>
   </si>
   <si>
@@ -655,6 +676,45 @@
   </si>
   <si>
     <t>TC4424EPA-ND</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
+    <t>R10,13,23,24,50,51,57,58</t>
+  </si>
+  <si>
+    <t>Q1,2,5,6,7,8</t>
+  </si>
+  <si>
+    <t>D9,10</t>
+  </si>
+  <si>
+    <t>LED1,2,5,6</t>
+  </si>
+  <si>
+    <t>R25,27</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>R11,14,35,37,48,49,55,56</t>
+  </si>
+  <si>
+    <t>R9,12,26,28</t>
+  </si>
+  <si>
+    <t>C11,20</t>
+  </si>
+  <si>
+    <t>A105963CT-ND</t>
+  </si>
+  <si>
+    <t>RES 680 OHM 0.6W 1% AXIAL</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
   </si>
 </sst>
 </file>
@@ -664,7 +724,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -727,6 +787,11 @@
       <color indexed="81"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Liberation Sans"/>
     </font>
   </fonts>
   <fills count="7">
@@ -828,7 +893,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -875,8 +940,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -943,20 +1010,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="48">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1001,6 +1077,8 @@
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1339,31 +1417,31 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="69.83203125" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="53.1640625" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
-    <col min="12" max="12" width="47.83203125" customWidth="1"/>
-    <col min="13" max="13" width="27.33203125" customWidth="1"/>
-    <col min="14" max="14" width="28" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="28" customWidth="1"/>
+    <col min="13" max="13" width="47.83203125" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" customWidth="1"/>
+    <col min="15" max="15" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="17" thickBot="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1375,34 +1453,37 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="23" t="s">
-        <v>181</v>
-      </c>
       <c r="N1" s="23" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" thickBot="1">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -1414,23 +1495,24 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4" t="str">
-        <f>IF(NOT(I2=""),A2&amp;","&amp;I2,"")</f>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4" t="str">
+        <f>IF(NOT(J2=""),A2&amp;","&amp;J2,"")</f>
         <v/>
       </c>
-      <c r="N2" t="str">
+      <c r="O2" t="str">
         <f>A2&amp;"x "&amp;C2</f>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="27" thickBot="1">
       <c r="A3" s="21">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
@@ -1441,42 +1523,43 @@
       <c r="E3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="5">
+      <c r="K3" s="5">
         <v>1.62</v>
       </c>
-      <c r="K3" s="6">
-        <f t="shared" ref="K3:K10" si="0">J3*A3</f>
+      <c r="L3" s="6">
+        <f t="shared" ref="L3:L10" si="0">K3*A3</f>
         <v>1.62</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4" t="str">
-        <f t="shared" ref="M3:M50" si="1">IF(NOT(I3=""),A3&amp;","&amp;I3,"")</f>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4" t="str">
+        <f t="shared" ref="N3:N50" si="1">IF(NOT(J3=""),A3&amp;","&amp;J3,"")</f>
         <v>1,478-1842-ND</v>
       </c>
-      <c r="N3" t="str">
+      <c r="O3" t="str">
         <f>"Capacitor - " &amp;A3&amp;"x "&amp;C3</f>
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="17" thickBot="1">
       <c r="A4" s="21">
         <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
@@ -1487,42 +1570,43 @@
       <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <v>15</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>0.66</v>
       </c>
-      <c r="K4" s="6">
+      <c r="L4" s="6">
         <f t="shared" si="0"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4" t="str">
+      <c r="M4" s="4"/>
+      <c r="N4" s="4" t="str">
         <f t="shared" si="1"/>
         <v>5,399-4288-ND</v>
       </c>
-      <c r="N4" t="str">
-        <f t="shared" ref="N4:N10" si="2">"Capacitor - " &amp;A4&amp;"x "&amp;C4</f>
+      <c r="O4" t="str">
+        <f t="shared" ref="O4:O10" si="2">"Capacitor - " &amp;A4&amp;"x "&amp;C4</f>
         <v>Capacitor - 5x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="17" thickBot="1">
       <c r="A5" s="21">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>23</v>
@@ -1533,42 +1617,43 @@
       <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
         <v>17</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="5">
         <v>0.22</v>
       </c>
-      <c r="K5" s="6">
+      <c r="L5" s="6">
         <f t="shared" si="0"/>
         <v>1.54</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4" t="str">
+      <c r="M5" s="4"/>
+      <c r="N5" s="4" t="str">
         <f t="shared" si="1"/>
         <v>7,399-4264-ND</v>
       </c>
-      <c r="N5" t="str">
+      <c r="O5" t="str">
         <f t="shared" si="2"/>
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="27" thickBot="1">
       <c r="A6" s="21">
         <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>27</v>
@@ -1579,42 +1664,43 @@
       <c r="E6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
         <v>2</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>1.65</v>
       </c>
-      <c r="K6" s="6">
+      <c r="L6" s="6">
         <f t="shared" si="0"/>
         <v>1.65</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4" t="str">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,478-1910-ND</v>
       </c>
-      <c r="N6" t="str">
+      <c r="O6" t="str">
         <f t="shared" si="2"/>
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="27" thickBot="1">
       <c r="A7" s="21">
         <f t="shared" ref="A7:A9" si="3">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>31</v>
@@ -1625,42 +1711,43 @@
       <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
         <v>2</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="5">
+      <c r="K7" s="5">
         <v>0.38</v>
       </c>
-      <c r="K7" s="6">
+      <c r="L7" s="6">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4" t="str">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,445-5312-ND</v>
       </c>
-      <c r="N7" t="str">
+      <c r="O7" t="str">
         <f t="shared" si="2"/>
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="17" thickBot="1">
       <c r="A8" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>36</v>
@@ -1671,42 +1758,43 @@
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
         <v>3</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="5">
+      <c r="K8" s="5">
         <v>0.31</v>
       </c>
-      <c r="K8" s="6">
+      <c r="L8" s="6">
         <f t="shared" si="0"/>
         <v>0.31</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4" t="str">
+      <c r="M8" s="4"/>
+      <c r="N8" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,399-4148-ND</v>
       </c>
-      <c r="N8" t="str">
+      <c r="O8" t="str">
         <f t="shared" si="2"/>
         <v>Capacitor - 1x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="17" thickBot="1">
       <c r="A9" s="21">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>40</v>
@@ -1717,80 +1805,82 @@
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
         <v>4</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="5">
+      <c r="K9" s="5">
         <v>0.79</v>
       </c>
-      <c r="K9" s="6">
+      <c r="L9" s="6">
         <f t="shared" si="0"/>
         <v>2.37</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4" t="str">
+      <c r="M9" s="4"/>
+      <c r="N9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>3,399-9714-ND</v>
       </c>
-      <c r="N9" t="str">
+      <c r="O9" t="str">
         <f t="shared" si="2"/>
         <v>Capacitor - 3x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="17" thickBot="1">
       <c r="A10" s="21">
         <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="J10" s="5">
+      <c r="I10" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K10" s="5">
         <v>0.25</v>
       </c>
-      <c r="K10" s="6">
+      <c r="L10" s="6">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4" t="str">
+      <c r="M10" s="4"/>
+      <c r="N10" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,399-4243-ND</v>
       </c>
-      <c r="N10" t="str">
+      <c r="O10" t="str">
         <f t="shared" si="2"/>
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="17" thickBot="1">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -1799,16 +1889,17 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4" t="str">
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="17" thickBot="1">
       <c r="A12" s="18"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -1817,25 +1908,26 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4" t="str">
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="40" thickBot="1">
       <c r="A13" s="21">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>44</v>
@@ -1843,45 +1935,46 @@
       <c r="E13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="I13" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="5">
+      <c r="K13" s="5">
         <v>0.34</v>
       </c>
-      <c r="K13" s="6">
-        <f>J13*A13</f>
+      <c r="L13" s="6">
+        <f>K13*A13</f>
         <v>0.34</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4" t="str">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,1N5919BGOS-ND</v>
       </c>
-      <c r="N13" t="str">
+      <c r="O13" t="str">
         <f>"Diode - " &amp;A13&amp;"x "&amp;C13</f>
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="40" thickBot="1">
       <c r="A14" s="21">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>50</v>
@@ -1889,82 +1982,84 @@
       <c r="E14" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
         <v>18</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="5">
+      <c r="K14" s="5">
         <v>0.27</v>
       </c>
-      <c r="K14" s="6">
-        <f>J14*A14</f>
+      <c r="L14" s="6">
+        <f>K14*A14</f>
         <v>3.24</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4" t="str">
+      <c r="M14" s="4"/>
+      <c r="N14" s="4" t="str">
         <f t="shared" si="1"/>
         <v>12,1N5818-TPCT-ND</v>
       </c>
-      <c r="N14" t="str">
-        <f t="shared" ref="N14:N16" si="4">"Diode - " &amp;A14&amp;"x "&amp;C14</f>
+      <c r="O14" t="str">
+        <f t="shared" ref="O14:O16" si="4">"Diode - " &amp;A14&amp;"x "&amp;C14</f>
         <v>Diode - 12x 1N5818-TP Schottky</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="17" thickBot="1">
       <c r="A15" s="21">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="J15" s="5">
+      <c r="I15" s="3"/>
+      <c r="J15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K15" s="5">
         <v>0.47</v>
       </c>
-      <c r="K15" s="6">
-        <f>J15*A15</f>
+      <c r="L15" s="6">
+        <f>K15*A15</f>
         <v>3.76</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4" t="str">
+      <c r="M15" s="4"/>
+      <c r="N15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>8,160-1139-ND</v>
       </c>
-      <c r="N15" t="str">
+      <c r="O15" t="str">
         <f t="shared" si="4"/>
         <v>Diode - 8x LED-Red</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="40" thickBot="1">
       <c r="A16" s="21">
         <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>54</v>
@@ -1975,36 +2070,37 @@
       <c r="E16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3">
         <v>13</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="5">
+      <c r="K16" s="5">
         <v>0.11</v>
       </c>
-      <c r="K16" s="6">
-        <f>J16*A16</f>
+      <c r="L16" s="6">
+        <f>K16*A16</f>
         <v>0.44</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4" t="str">
+      <c r="M16" s="4"/>
+      <c r="N16" s="4" t="str">
         <f t="shared" si="1"/>
         <v>4,1N4004-TPMSCT-ND</v>
       </c>
-      <c r="N16" t="str">
+      <c r="O16" t="str">
         <f t="shared" si="4"/>
         <v>Diode - 4x 1N4004</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="17" thickBot="1">
       <c r="A17" s="18"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -2013,20 +2109,21 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4" t="str">
+      <c r="L17" s="3"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N17" t="str">
-        <f t="shared" ref="N17:N45" si="5">A17&amp;"x "&amp;C17</f>
+      <c r="O17" t="str">
+        <f t="shared" ref="O17:O45" si="5">A17&amp;"x "&amp;C17</f>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="17" thickBot="1">
       <c r="A18" s="19"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -2035,20 +2132,21 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="9"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="4" t="str">
+      <c r="M18" s="3"/>
+      <c r="N18" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N18" t="str">
+      <c r="O18" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="17" thickBot="1">
       <c r="A19" s="18"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -2057,25 +2155,26 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="2"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4" t="str">
+      <c r="L19" s="3"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N19" t="str">
+      <c r="O19" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="27" thickBot="1">
       <c r="A20" s="21">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>58</v>
@@ -2086,36 +2185,37 @@
       <c r="E20" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
         <v>1</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J20" s="5">
+      <c r="K20" s="5">
         <v>0.72</v>
       </c>
-      <c r="K20" s="6">
-        <f>J20*A20</f>
+      <c r="L20" s="6">
+        <f>K20*A20</f>
         <v>0.72</v>
       </c>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4" t="str">
+      <c r="M20" s="4"/>
+      <c r="N20" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,P7307-ND</v>
       </c>
-      <c r="N20" t="str">
+      <c r="O20" t="str">
         <f t="shared" si="5"/>
         <v>1x Surge Protection</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="17" thickBot="1">
       <c r="A21" s="18"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
@@ -2124,143 +2224,147 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="2"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4" t="str">
+      <c r="L21" s="3"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N21" t="str">
+      <c r="O21" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="40" thickBot="1">
       <c r="A22" s="21">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K22" s="3">
         <v>0.40200000000000002</v>
       </c>
-      <c r="K22" s="6">
-        <f>J22*A22</f>
+      <c r="L22" s="6">
+        <f>K22*A22</f>
         <v>5.6280000000000001</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="M22" s="4" t="str">
+      <c r="M22" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="N22" s="4" t="str">
         <f t="shared" si="1"/>
         <v>14,ED2561-ND</v>
       </c>
-      <c r="N22" t="str">
+      <c r="O22" t="str">
         <f>A22&amp;"x "&amp;C22</f>
         <v>14x Dual Terminal Block</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="17" thickBot="1">
       <c r="A23" s="21">
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J23" s="5">
+      <c r="I23" s="3"/>
+      <c r="J23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K23" s="5">
         <v>0.1</v>
       </c>
-      <c r="K23" s="6">
-        <f>J23*A23</f>
+      <c r="L23" s="6">
+        <f>K23*A23</f>
         <v>0.5</v>
       </c>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4" t="str">
+      <c r="M23" s="4"/>
+      <c r="N23" s="4" t="str">
         <f t="shared" si="1"/>
         <v>5,3M9580-ND</v>
       </c>
-      <c r="N23" t="str">
+      <c r="O23" t="str">
         <f t="shared" si="5"/>
         <v>5x Jumper</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="40" thickBot="1">
       <c r="A24" s="21">
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="3">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3">
         <v>1</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="H24" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J24" s="6">
+        <v>156</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K24" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="K24" s="6">
-        <f>J24*A24</f>
+      <c r="L24" s="6">
+        <f>K24*A24</f>
         <v>0.56000000000000005</v>
       </c>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4" t="str">
+      <c r="M24" s="4"/>
+      <c r="N24" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,S1012EC-40-ND</v>
       </c>
-      <c r="N24" t="str">
+      <c r="O24" t="str">
         <f t="shared" si="5"/>
         <v>1x 40 POS 0.100 Pin Header</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="17" thickBot="1">
       <c r="A25" s="18"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
@@ -2269,20 +2373,21 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4" t="str">
+      <c r="I25" s="3"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N25" t="str">
+      <c r="O25" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="17" thickBot="1">
       <c r="A26" s="18"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
@@ -2291,66 +2396,68 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4" t="str">
+      <c r="I26" s="3"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="N26" t="str">
+      <c r="O26" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="27" thickBot="1">
       <c r="A27" s="21">
         <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="3">
+        <v>101</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3">
         <v>8</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="J27" s="6">
+      <c r="I27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K27" s="6">
         <v>1.51</v>
       </c>
-      <c r="K27" s="6">
-        <f>J27*A27</f>
+      <c r="L27" s="6">
+        <f>K27*A27</f>
         <v>12.08</v>
       </c>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4" t="str">
+      <c r="M27" s="4"/>
+      <c r="N27" s="4" t="str">
         <f t="shared" si="1"/>
         <v>8,497-5896-5-ND</v>
       </c>
-      <c r="N27" t="str">
+      <c r="O27" t="str">
         <f t="shared" si="5"/>
         <v>8x 62A MOSFET N-CH</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="17" thickBot="1">
       <c r="A28" s="18"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
@@ -2359,16 +2466,17 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="2"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4" t="str">
+      <c r="L28" s="3"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="17" thickBot="1">
       <c r="A29" s="18"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
@@ -2377,22 +2485,23 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="3"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4" t="str">
+      <c r="L29" s="3"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="17" thickBot="1">
       <c r="A30" s="21">
         <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>66</v>
@@ -2401,42 +2510,43 @@
         <v>67</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="3">
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
         <v>7</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="I30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J30" s="5">
+      <c r="K30" s="5">
         <v>0.08</v>
       </c>
-      <c r="K30" s="6">
-        <f t="shared" ref="K30:K38" si="6">J30*A30</f>
+      <c r="L30" s="6">
+        <f t="shared" ref="L30:L38" si="6">K30*A30</f>
         <v>0.4</v>
       </c>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4" t="str">
+      <c r="M30" s="4"/>
+      <c r="N30" s="4" t="str">
         <f t="shared" si="1"/>
         <v>5,10.0KXBK-ND</v>
       </c>
-      <c r="N30" t="str">
+      <c r="O30" t="str">
         <f>"Resistor - " &amp; A30&amp;"x "&amp;C30</f>
         <v>Resistor - 5x 10k</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="17" thickBot="1">
       <c r="A31" s="21">
         <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>71</v>
@@ -2445,349 +2555,353 @@
         <v>72</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="3">
+      <c r="F31" s="3"/>
+      <c r="G31" s="3">
         <v>32</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="I31" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J31" s="5">
+      <c r="K31" s="5">
         <v>0.06</v>
       </c>
-      <c r="K31" s="6">
+      <c r="L31" s="6">
         <f t="shared" si="6"/>
         <v>0.72</v>
       </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4" t="str">
+      <c r="M31" s="4"/>
+      <c r="N31" s="4" t="str">
         <f t="shared" si="1"/>
         <v>12,1.00KXBK-ND</v>
       </c>
-      <c r="N31" t="str">
-        <f t="shared" ref="N31:N38" si="7">"Resistor - " &amp; A31&amp;"x "&amp;C31</f>
+      <c r="O31" t="str">
+        <f t="shared" ref="O31:O38" si="7">"Resistor - " &amp; A31&amp;"x "&amp;C31</f>
         <v>Resistor - 12x 1k</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="40" thickBot="1">
       <c r="A32" s="21">
         <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C32" s="14">
         <v>680</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>116</v>
+        <v>207</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="14">
-        <v>17</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J32" s="15">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="K32" s="6">
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="I32" s="7"/>
+      <c r="J32" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K32" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="L32" s="6">
         <f t="shared" si="6"/>
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="M32" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>8,2.43KXBK-ND</v>
-      </c>
-      <c r="N32" t="str">
+        <v>1.76</v>
+      </c>
+      <c r="M32" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="N32" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>8,A105963CT-ND</v>
+      </c>
+      <c r="O32" t="str">
         <f t="shared" si="7"/>
         <v>Resistor - 8x 680</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="40" thickBot="1">
       <c r="A33" s="21">
         <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C33" s="3">
         <v>470</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3">
+        <v>9</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3">
-        <v>9</v>
-      </c>
-      <c r="G33" s="3" t="s">
+      <c r="J33" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H33" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J33" s="5">
+      <c r="K33" s="5">
         <v>0.11</v>
       </c>
-      <c r="K33" s="6">
+      <c r="L33" s="6">
         <f t="shared" si="6"/>
         <v>0.66</v>
       </c>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4" t="str">
+      <c r="M33" s="4"/>
+      <c r="N33" s="4" t="str">
         <f t="shared" si="1"/>
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
-      <c r="N33" t="str">
+      <c r="O33" t="str">
         <f t="shared" si="7"/>
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="40" thickBot="1">
       <c r="A34" s="21">
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3">
+        <v>3</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F34" s="3">
-        <v>3</v>
-      </c>
-      <c r="G34" s="3" t="s">
+      <c r="J34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J34" s="5">
+      <c r="K34" s="5">
         <v>1.92</v>
       </c>
-      <c r="K34" s="6">
+      <c r="L34" s="6">
         <f t="shared" si="6"/>
         <v>3.84</v>
       </c>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4" t="str">
+      <c r="M34" s="4"/>
+      <c r="N34" s="4" t="str">
         <f t="shared" si="1"/>
         <v>2,985-1047-1-ND</v>
       </c>
-      <c r="N34" t="str">
+      <c r="O34" t="str">
         <f t="shared" si="7"/>
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="17" thickBot="1">
       <c r="A35" s="21">
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J35" s="5">
+      <c r="K35" s="5">
         <v>0.46</v>
       </c>
-      <c r="K35" s="6">
+      <c r="L35" s="6">
         <f t="shared" si="6"/>
         <v>0.46</v>
       </c>
-      <c r="L35" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="M35" s="4" t="str">
+      <c r="M35" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N35" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,3.9KADCT-ND</v>
       </c>
-      <c r="N35" t="str">
+      <c r="O35" t="str">
         <f t="shared" si="7"/>
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="17" thickBot="1">
       <c r="A36" s="21">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3">
-        <v>1</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J36" s="5">
+      <c r="K36" s="5">
         <v>0.46</v>
       </c>
-      <c r="K36" s="6">
+      <c r="L36" s="6">
         <f t="shared" si="6"/>
         <v>0.46</v>
       </c>
-      <c r="L36" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="M36" s="4" t="str">
+      <c r="M36" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N36" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,1KADCT-ND</v>
       </c>
-      <c r="N36" t="str">
+      <c r="O36" t="str">
         <f t="shared" si="7"/>
         <v>Resistor - 1x 0.1% 1.0k</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="17" thickBot="1">
       <c r="A37" s="21">
         <f t="shared" ref="A37:A38" si="8">LEN(B37)-LEN(SUBSTITUTE(B37,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3">
+        <v>17</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="J37" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3">
-        <v>17</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J37" s="5">
+      <c r="K37" s="5">
         <v>0.1</v>
       </c>
-      <c r="K37" s="6">
+      <c r="L37" s="6">
         <f t="shared" si="6"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4" t="str">
+      <c r="M37" s="4"/>
+      <c r="N37" s="4" t="str">
         <f t="shared" si="1"/>
         <v>12,100KXBK-ND</v>
       </c>
-      <c r="N37" t="str">
+      <c r="O37" t="str">
         <f t="shared" si="7"/>
         <v>Resistor - 12x 100k</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="17" thickBot="1">
       <c r="A38" s="21">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C38" s="3">
         <v>160</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3">
+        <v>4</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3">
-        <v>4</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J38" s="5">
+      <c r="K38" s="5">
         <v>0.27</v>
       </c>
-      <c r="K38" s="6">
+      <c r="L38" s="6">
         <f t="shared" si="6"/>
         <v>1.08</v>
       </c>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4" t="str">
+      <c r="M38" s="4"/>
+      <c r="N38" s="4" t="str">
         <f t="shared" si="1"/>
         <v>4,160YCT-ND</v>
       </c>
-      <c r="N38" t="str">
+      <c r="O38" t="str">
         <f t="shared" si="7"/>
         <v>Resistor - 4x 160</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="17" thickBot="1">
       <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
@@ -2796,16 +2910,17 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="2"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4" t="str">
+      <c r="L39" s="3"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="17" thickBot="1">
       <c r="A40" s="18"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3"/>
@@ -2814,352 +2929,363 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="2"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4" t="str">
+      <c r="L40" s="3"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="27" thickBot="1">
       <c r="A41" s="21">
         <v>1</v>
       </c>
       <c r="B41" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="F41" s="3"/>
+      <c r="G41" s="3">
+        <v>2</v>
+      </c>
+      <c r="H41" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F41" s="3">
-        <v>2</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J41" s="5">
+      <c r="I41" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K41" s="5">
         <v>1.68</v>
       </c>
-      <c r="K41" s="6">
-        <f>J41*A41</f>
+      <c r="L41" s="6">
+        <f>K41*A41</f>
         <v>1.68</v>
       </c>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4" t="str">
+      <c r="M41" s="4"/>
+      <c r="N41" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,LM2940T-5.0/NOPB</v>
       </c>
-      <c r="N41" t="str">
+      <c r="O41" t="str">
         <f t="shared" si="5"/>
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="40" thickBot="1">
       <c r="A42" s="21">
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" s="3">
+        <v>122</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3">
         <v>1</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H42" s="3"/>
-      <c r="I42" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J42" s="6">
+      <c r="H42" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="J42" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K42" s="6">
         <v>15.41</v>
       </c>
-      <c r="K42" s="6">
-        <f>J42*A42</f>
+      <c r="L42" s="6">
+        <f>K42*A42</f>
         <v>15.41</v>
       </c>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4" t="str">
+      <c r="M42" s="4"/>
+      <c r="N42" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,MPX4250AP-ND</v>
       </c>
-      <c r="N42" t="str">
+      <c r="O42" t="str">
         <f t="shared" si="5"/>
         <v>1x 1-Bar MAP sensor</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26">
+    <row r="43" spans="1:15" ht="27" thickBot="1">
+      <c r="A43" s="24">
         <v>2</v>
       </c>
       <c r="B43" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="F43" s="14"/>
+      <c r="G43" s="14">
+        <v>2</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="F43" s="14">
-        <v>2</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="J43" s="27">
+      <c r="K43" s="25">
         <v>2.92</v>
       </c>
-      <c r="K43" s="6">
-        <f>J43*A43</f>
+      <c r="L43" s="6">
+        <f>K43*A43</f>
         <v>5.84</v>
       </c>
-      <c r="L43" s="13"/>
-      <c r="M43" s="4" t="str">
+      <c r="M43" s="13"/>
+      <c r="N43" s="4" t="str">
         <f t="shared" si="1"/>
         <v>2,TC4424EPA-ND</v>
       </c>
-      <c r="N43" t="str">
+      <c r="O43" t="str">
         <f t="shared" si="5"/>
         <v>2x TC4424EPA</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="27" thickBot="1">
       <c r="A44" s="21">
         <v>1</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F44" s="3"/>
-      <c r="G44" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="G44" s="3"/>
       <c r="H44" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="I44" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I44" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J44" s="6">
+      <c r="J44" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K44" s="6">
         <v>1.61</v>
       </c>
-      <c r="K44" s="6">
-        <f>J44*A44</f>
+      <c r="L44" s="6">
+        <f>K44*A44</f>
         <v>1.61</v>
       </c>
-      <c r="L44" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="M44" s="4" t="str">
+      <c r="M44" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="N44" s="4" t="str">
         <f t="shared" si="1"/>
         <v>1,24LC512-I/P-ND</v>
       </c>
-      <c r="N44" t="str">
+      <c r="O44" t="str">
         <f t="shared" si="5"/>
         <v>1x 512Kb EEPROM</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="17" thickBot="1">
       <c r="A45" s="21">
         <v>3</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J45" s="6">
+      <c r="H45" s="3"/>
+      <c r="I45" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K45" s="6">
         <v>0.5</v>
       </c>
-      <c r="K45" s="6">
-        <f>J45*A45</f>
+      <c r="L45" s="6">
+        <f>K45*A45</f>
         <v>1.5</v>
       </c>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4" t="str">
+      <c r="M45" s="4"/>
+      <c r="N45" s="4" t="str">
         <f t="shared" si="1"/>
         <v>3,AE10011-ND</v>
       </c>
-      <c r="N45" t="str">
+      <c r="O45" t="str">
         <f t="shared" si="5"/>
         <v>3x IC Socket</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="17" thickBot="1">
       <c r="A46" s="18"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="4"/>
+      <c r="F46" s="3"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="11"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="1"/>
       <c r="L46" s="11"/>
-      <c r="M46" s="4" t="str">
+      <c r="M46" s="11"/>
+      <c r="N46" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="17" thickBot="1">
       <c r="A47" s="18">
         <v>0</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
-      <c r="F47" s="3">
+      <c r="F47" s="3"/>
+      <c r="G47" s="3">
         <v>1</v>
       </c>
-      <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6">
-        <f>J47*A47</f>
+      <c r="I47" s="3"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6">
+        <f>K47*A47</f>
         <v>0</v>
       </c>
-      <c r="L47" s="11"/>
-      <c r="M47" s="4" t="str">
+      <c r="M47" s="11"/>
+      <c r="N47" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="17" thickBot="1">
       <c r="A48" s="18"/>
       <c r="B48" s="4"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="4"/>
+      <c r="F48" s="3"/>
       <c r="G48" s="4"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="11"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="1"/>
       <c r="L48" s="11"/>
-      <c r="M48" s="4" t="str">
+      <c r="M48" s="11"/>
+      <c r="N48" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="17" thickBot="1">
       <c r="A49" s="18"/>
       <c r="B49" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="4"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="9"/>
       <c r="H49" s="4"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4" t="str">
+      <c r="I49" s="4"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="17" thickBot="1">
       <c r="A50" s="18">
         <v>1</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="3">
+      <c r="F50" s="3"/>
+      <c r="G50" s="3">
         <v>1</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="H50" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="6">
+        <v>108</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J50" s="3"/>
+      <c r="K50" s="6">
         <v>15</v>
       </c>
-      <c r="K50" s="6">
-        <f>J50*A50</f>
+      <c r="L50" s="6">
+        <f>K50*A50</f>
         <v>15</v>
       </c>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4" t="str">
+      <c r="M50" s="4"/>
+      <c r="N50" s="4" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="17" thickBot="1">
       <c r="A51" s="18">
         <v>1</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -3167,61 +3293,2015 @@
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="J51" s="3">
+      <c r="I51" s="3"/>
+      <c r="J51" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K51" s="3">
         <v>61.65</v>
       </c>
-      <c r="K51" s="6"/>
-      <c r="L51" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L51" s="6"/>
+      <c r="M51" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="17" thickBot="1">
       <c r="A52" s="18"/>
       <c r="B52" s="4"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="I52" s="25"/>
-      <c r="J52" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K52" s="12">
-        <f>SUM(K2:K51)</f>
-        <v>89.668000000000006</v>
-      </c>
-      <c r="L52" s="11" t="s">
-        <v>107</v>
+      <c r="F52" s="26"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="J52" s="30"/>
+      <c r="K52" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L52" s="12">
+        <f>SUM(L2:L51)</f>
+        <v>90.308000000000007</v>
+      </c>
+      <c r="M52" s="11" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="I52:J52"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1"/>
-    <hyperlink ref="I6" r:id="rId2"/>
-    <hyperlink ref="I7" r:id="rId3"/>
-    <hyperlink ref="I8" r:id="rId4"/>
-    <hyperlink ref="I14" r:id="rId5"/>
-    <hyperlink ref="I20" r:id="rId6"/>
-    <hyperlink ref="I30" r:id="rId7"/>
-    <hyperlink ref="I34" r:id="rId8"/>
-    <hyperlink ref="I35" r:id="rId9"/>
-    <hyperlink ref="I36" r:id="rId10"/>
-    <hyperlink ref="I37" r:id="rId11"/>
-    <hyperlink ref="I42" r:id="rId12"/>
+    <hyperlink ref="J3" r:id="rId1"/>
+    <hyperlink ref="J6" r:id="rId2"/>
+    <hyperlink ref="J7" r:id="rId3"/>
+    <hyperlink ref="J8" r:id="rId4"/>
+    <hyperlink ref="J14" r:id="rId5"/>
+    <hyperlink ref="J20" r:id="rId6"/>
+    <hyperlink ref="J30" r:id="rId7"/>
+    <hyperlink ref="J34" r:id="rId8"/>
+    <hyperlink ref="J35" r:id="rId9"/>
+    <hyperlink ref="J36" r:id="rId10"/>
+    <hyperlink ref="J37" r:id="rId11"/>
+    <hyperlink ref="J42" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="36" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="35" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId13"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32:K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="53.1640625" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="28" customWidth="1"/>
+    <col min="13" max="13" width="47.83203125" customWidth="1"/>
+    <col min="14" max="14" width="27.33203125" customWidth="1"/>
+    <col min="15" max="15" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="17" thickBot="1">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" thickBot="1">
+      <c r="A2" s="18"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4" t="str">
+        <f>IF(NOT(J2=""),A2&amp;","&amp;J2,"")</f>
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <f>A2&amp;"x "&amp;C2</f>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="27" thickBot="1">
+      <c r="A3" s="21">
+        <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1.62</v>
+      </c>
+      <c r="L3" s="6">
+        <f t="shared" ref="L3:L10" si="0">K3*A3</f>
+        <v>1.62</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4" t="str">
+        <f t="shared" ref="N3:N50" si="1">IF(NOT(J3=""),A3&amp;","&amp;J3,"")</f>
+        <v>1,478-1842-ND</v>
+      </c>
+      <c r="O3" t="str">
+        <f>"Capacitor - " &amp;A3&amp;"x "&amp;C3</f>
+        <v>Capacitor - 1x 10uF</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17" thickBot="1">
+      <c r="A4" s="21">
+        <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
+        <v>15</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="L4" s="6">
+        <f t="shared" si="0"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>5,399-4288-ND</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" ref="O4:O10" si="2">"Capacitor - " &amp;A4&amp;"x "&amp;C4</f>
+        <v>Capacitor - 5x 0.22uF</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="17" thickBot="1">
+      <c r="A5" s="21">
+        <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3">
+        <v>17</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="L5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.54</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>7,399-4264-ND</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 7x 0.1uF / 100nF</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="27" thickBot="1">
+      <c r="A6" s="21">
+        <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="5">
+        <v>1.65</v>
+      </c>
+      <c r="L6" s="6">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,478-1910-ND</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 1x 47uF</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="27" thickBot="1">
+      <c r="A7" s="21">
+        <f t="shared" ref="A7:A9" si="3">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0.38</v>
+      </c>
+      <c r="L7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,445-5312-ND</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 1x 0.33uF</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="17" thickBot="1">
+      <c r="A8" s="21">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0.31</v>
+      </c>
+      <c r="L8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.31</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,399-4148-ND</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 1x 0.01uF</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="16" thickBot="1">
+      <c r="A9" s="21">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0.79</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" si="0"/>
+        <v>1.58</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>2,399-9714-ND</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 2x 1uF</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="17" thickBot="1">
+      <c r="A10" s="21">
+        <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,399-4243-ND</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor - 1x 4.7nF</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="17" thickBot="1">
+      <c r="A11" s="18"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="17" thickBot="1">
+      <c r="A12" s="18"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="40" thickBot="1">
+      <c r="A13" s="21">
+        <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.34</v>
+      </c>
+      <c r="L13" s="6">
+        <f>K13*A13</f>
+        <v>0.34</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,1N5919BGOS-ND</v>
+      </c>
+      <c r="O13" t="str">
+        <f>"Diode - " &amp;A13&amp;"x "&amp;C13</f>
+        <v>Diode - 1x 1N5919BG Zener</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="40" thickBot="1">
+      <c r="A14" s="21">
+        <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
+        <v>18</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="L14" s="6">
+        <f>K14*A14</f>
+        <v>3.24</v>
+      </c>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>12,1N5818-TPCT-ND</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" ref="O14:O16" si="4">"Diode - " &amp;A14&amp;"x "&amp;C14</f>
+        <v>Diode - 12x 1N5818-TP Schottky</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="17" thickBot="1">
+      <c r="A15" s="21">
+        <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
+        <v>4</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0.47</v>
+      </c>
+      <c r="L15" s="6">
+        <f>K15*A15</f>
+        <v>1.88</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>4,160-1139-ND</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="4"/>
+        <v>Diode - 4x LED-Red</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="40" thickBot="1">
+      <c r="A16" s="21">
+        <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
+        <v>2</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3">
+        <v>13</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="L16" s="6">
+        <f>K16*A16</f>
+        <v>0.22</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>2,1N4004-TPMSCT-ND</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="4"/>
+        <v>Diode - 2x 1N4004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="17" thickBot="1">
+      <c r="A17" s="18"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" ref="O17:O45" si="5">A17&amp;"x "&amp;C17</f>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="17" thickBot="1">
+      <c r="A18" s="19"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="17" thickBot="1">
+      <c r="A19" s="18"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="27" thickBot="1">
+      <c r="A20" s="21">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="L20" s="6">
+        <f>K20*A20</f>
+        <v>0.72</v>
+      </c>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,P7307-ND</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="5"/>
+        <v>1x Surge Protection</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="17" thickBot="1">
+      <c r="A21" s="18"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="40" thickBot="1">
+      <c r="A22" s="21">
+        <v>14</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="L22" s="6">
+        <f>K22*A22</f>
+        <v>5.6280000000000001</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="N22" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>14,ED2561-ND</v>
+      </c>
+      <c r="O22" t="str">
+        <f>A22&amp;"x "&amp;C22</f>
+        <v>14x Dual Terminal Block</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="17" thickBot="1">
+      <c r="A23" s="21">
+        <v>5</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="L23" s="6">
+        <f>K23*A23</f>
+        <v>0.5</v>
+      </c>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>5,3M9580-ND</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="5"/>
+        <v>5x Jumper</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="40" thickBot="1">
+      <c r="A24" s="21">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K24" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L24" s="6">
+        <f>K24*A24</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,S1012EC-40-ND</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="5"/>
+        <v>1x 40 POS 0.100 Pin Header</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="17" thickBot="1">
+      <c r="A25" s="18"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="17" thickBot="1">
+      <c r="A26" s="18"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">x </v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="27" thickBot="1">
+      <c r="A27" s="21">
+        <v>6</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3">
+        <v>8</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K27" s="6">
+        <v>1.51</v>
+      </c>
+      <c r="L27" s="6">
+        <f>K27*A27</f>
+        <v>9.06</v>
+      </c>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>6,497-5896-5-ND</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="5"/>
+        <v>6x 62A MOSFET N-CH</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="17" thickBot="1">
+      <c r="A28" s="18"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="17" thickBot="1">
+      <c r="A29" s="18"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="17" thickBot="1">
+      <c r="A30" s="21">
+        <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
+        <v>5</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3">
+        <v>7</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K30" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" ref="L30:L38" si="6">K30*A30</f>
+        <v>0.4</v>
+      </c>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>5,10.0KXBK-ND</v>
+      </c>
+      <c r="O30" t="str">
+        <f>"Resistor - " &amp; A30&amp;"x "&amp;C30</f>
+        <v>Resistor - 5x 10k</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="17" thickBot="1">
+      <c r="A31" s="21">
+        <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
+        <v>8</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3">
+        <v>32</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K31" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="6"/>
+        <v>0.48</v>
+      </c>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>8,1.00KXBK-ND</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" ref="O31:O38" si="7">"Resistor - " &amp; A31&amp;"x "&amp;C31</f>
+        <v>Resistor - 8x 1k</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="31" customHeight="1" thickBot="1">
+      <c r="A32" s="21">
+        <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
+        <v>4</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="C32" s="14">
+        <v>680</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="I32" s="7"/>
+      <c r="J32" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K32" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" si="6"/>
+        <v>0.88</v>
+      </c>
+      <c r="M32" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="N32" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>4,A105963CT-ND</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 4x 680</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="40" thickBot="1">
+      <c r="A33" s="21">
+        <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
+        <v>6</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="3">
+        <v>470</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3">
+        <v>9</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K33" s="5">
+        <v>0.11</v>
+      </c>
+      <c r="L33" s="6">
+        <f t="shared" si="6"/>
+        <v>0.66</v>
+      </c>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>6,RNF14FTD470RCT-ND</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 6x 470</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="40" thickBot="1">
+      <c r="A34" s="21">
+        <f>LEN(B34)-LEN(SUBSTITUTE(B34,",",""))+1</f>
+        <v>2</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3">
+        <v>3</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K34" s="5">
+        <v>1.92</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="6"/>
+        <v>3.84</v>
+      </c>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>2,985-1047-1-ND</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 2x 0.1% 2.49k</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="17" thickBot="1">
+      <c r="A35" s="21">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K35" s="5">
+        <v>0.46</v>
+      </c>
+      <c r="L35" s="6">
+        <f t="shared" si="6"/>
+        <v>0.46</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N35" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,3.9KADCT-ND</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 1x 0.1% 3.9k</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="17" thickBot="1">
+      <c r="A36" s="21">
+        <v>1</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K36" s="5">
+        <v>0.46</v>
+      </c>
+      <c r="L36" s="6">
+        <f t="shared" si="6"/>
+        <v>0.46</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N36" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,1KADCT-ND</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 1x 0.1% 1.0k</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="17" thickBot="1">
+      <c r="A37" s="21">
+        <f t="shared" ref="A37:A38" si="8">LEN(B37)-LEN(SUBSTITUTE(B37,",",""))+1</f>
+        <v>8</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3">
+        <v>17</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K37" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="L37" s="6">
+        <f t="shared" si="6"/>
+        <v>0.8</v>
+      </c>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>8,100KXBK-ND</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 8x 100k</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="17" thickBot="1">
+      <c r="A38" s="21">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="C38" s="3">
+        <v>160</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3">
+        <v>4</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K38" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="L38" s="6">
+        <f t="shared" si="6"/>
+        <v>0.54</v>
+      </c>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>2,160YCT-ND</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="7"/>
+        <v>Resistor - 2x 160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="17" thickBot="1">
+      <c r="A39" s="18"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="17" thickBot="1">
+      <c r="A40" s="18"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="27" thickBot="1">
+      <c r="A41" s="21">
+        <v>1</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3">
+        <v>2</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K41" s="5">
+        <v>1.68</v>
+      </c>
+      <c r="L41" s="6">
+        <f>K41*A41</f>
+        <v>1.68</v>
+      </c>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,LM2940T-5.0/NOPB</v>
+      </c>
+      <c r="O41" t="str">
+        <f t="shared" si="5"/>
+        <v>1x LM2940T-5.0/NOPB</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="40" thickBot="1">
+      <c r="A42" s="21">
+        <v>1</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3">
+        <v>1</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" s="3"/>
+      <c r="J42" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K42" s="6">
+        <v>15.41</v>
+      </c>
+      <c r="L42" s="6">
+        <f>K42*A42</f>
+        <v>15.41</v>
+      </c>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,MPX4250AP-ND</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" si="5"/>
+        <v>1x 1-Bar MAP sensor</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="27" thickBot="1">
+      <c r="A43" s="21">
+        <v>1</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14">
+        <v>2</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="K43" s="25">
+        <v>2.92</v>
+      </c>
+      <c r="L43" s="6">
+        <f>K43*A43</f>
+        <v>2.92</v>
+      </c>
+      <c r="M43" s="13"/>
+      <c r="N43" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,TC4424EPA-ND</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" si="5"/>
+        <v>1x TC4424EPA</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="27" thickBot="1">
+      <c r="A44" s="21">
+        <v>1</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K44" s="6">
+        <v>1.61</v>
+      </c>
+      <c r="L44" s="6">
+        <f>K44*A44</f>
+        <v>1.61</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="N44" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>1,24LC512-I/P-ND</v>
+      </c>
+      <c r="O44" t="str">
+        <f t="shared" si="5"/>
+        <v>1x 512Kb EEPROM</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="17" thickBot="1">
+      <c r="A45" s="21">
+        <v>3</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="K45" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="L45" s="6">
+        <f>K45*A45</f>
+        <v>1.5</v>
+      </c>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>3,AE10011-ND</v>
+      </c>
+      <c r="O45" t="str">
+        <f t="shared" si="5"/>
+        <v>3x IC Socket</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="17" thickBot="1">
+      <c r="A46" s="18"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="17" thickBot="1">
+      <c r="A47" s="18">
+        <v>0</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3">
+        <v>1</v>
+      </c>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6">
+        <f>K47*A47</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="11"/>
+      <c r="N47" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="17" thickBot="1">
+      <c r="A48" s="18"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="17" thickBot="1">
+      <c r="A49" s="18"/>
+      <c r="B49" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="17" thickBot="1">
+      <c r="A50" s="18">
+        <v>1</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3">
+        <v>1</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J50" s="3"/>
+      <c r="K50" s="6">
+        <v>15</v>
+      </c>
+      <c r="L50" s="6">
+        <f>K50*A50</f>
+        <v>15</v>
+      </c>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="17" thickBot="1">
+      <c r="A51" s="18">
+        <v>1</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K51" s="3">
+        <v>61.65</v>
+      </c>
+      <c r="L51" s="6"/>
+      <c r="M51" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="17" thickBot="1">
+      <c r="A52" s="18"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="J52" s="30"/>
+      <c r="K52" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L52" s="12">
+        <f>SUM(L2:L51)</f>
+        <v>79.417999999999992</v>
+      </c>
+      <c r="M52" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I52:J52"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1"/>
+    <hyperlink ref="J6" r:id="rId2"/>
+    <hyperlink ref="J7" r:id="rId3"/>
+    <hyperlink ref="J8" r:id="rId4"/>
+    <hyperlink ref="J14" r:id="rId5"/>
+    <hyperlink ref="J20" r:id="rId6"/>
+    <hyperlink ref="J30" r:id="rId7"/>
+    <hyperlink ref="J34" r:id="rId8"/>
+    <hyperlink ref="J35" r:id="rId9"/>
+    <hyperlink ref="J36" r:id="rId10"/>
+    <hyperlink ref="J37" r:id="rId11"/>
+    <hyperlink ref="J42" r:id="rId12"/>
+  </hyperlinks>
+  <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="35" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId13"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>